<commit_message>
Add create category and create town to admin view!
</commit_message>
<xml_diff>
--- a/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="64">
   <si>
     <t>Days Commit in GitHub</t>
   </si>
@@ -208,9 +208,6 @@
   </si>
   <si>
     <t>YES</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
   <si>
     <t>NO</t>
@@ -688,7 +685,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -698,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1094,7 +1091,7 @@
         <v>28</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
@@ -1118,7 +1115,7 @@
         <v>28</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
@@ -1142,7 +1139,7 @@
         <v>28</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
@@ -1154,7 +1151,7 @@
         <v>28</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
@@ -1166,7 +1163,7 @@
         <v>28</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
@@ -1178,7 +1175,7 @@
         <v>28</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
@@ -1190,7 +1187,7 @@
         <v>28</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.25">
@@ -1202,7 +1199,7 @@
         <v>28</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.25">
@@ -1214,7 +1211,7 @@
         <v>28</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
@@ -1226,7 +1223,7 @@
         <v>28</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
@@ -1250,7 +1247,7 @@
         <v>28</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
@@ -1262,7 +1259,7 @@
         <v>28</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.25">
@@ -1274,7 +1271,7 @@
         <v>28</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="51" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">

</xml_diff>